<commit_message>
removed unnecessary files on github
</commit_message>
<xml_diff>
--- a/javu.xlsx
+++ b/javu.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Хуй</t>
   </si>
@@ -101,6 +100,12 @@
   </si>
   <si>
     <t>Кокол2</t>
+  </si>
+  <si>
+    <t>asasd</t>
+  </si>
+  <si>
+    <t>asdasd</t>
   </si>
 </sst>
 </file>
@@ -491,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +509,7 @@
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -529,7 +534,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -553,7 +558,7 @@
       </c>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -577,7 +582,7 @@
       </c>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -601,7 +606,7 @@
       </c>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -625,7 +630,7 @@
       </c>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -649,6 +654,16 @@
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>